<commit_message>
1. Update formAr/formN2 report 2. Display latest water/O2 on dashboard
</commit_message>
<xml_diff>
--- a/report_template/formAr.xlsx
+++ b/report_template/formAr.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27830"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\repo\gc\report_template\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\USER\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E7D8DB4-8818-498E-8608-8441F2D3DBB3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{483D9EEA-ADD6-4CBF-B7E6-68D9BBBAF2E5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-103" yWindow="-103" windowWidth="33120" windowHeight="18000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="LAR" sheetId="3" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">LAR!$A$1:$K$18</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">LAR!$A$1:$K$19</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -27,8 +27,6 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -36,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="37">
   <si>
     <t>分析報告</t>
   </si>
@@ -224,16 +222,53 @@
     </r>
     <phoneticPr fontId="5" type="noConversion"/>
   </si>
+  <si>
+    <t>H2O</t>
+  </si>
+  <si>
+    <t>O2</t>
+  </si>
+  <si>
+    <t>&lt; 80</t>
+  </si>
+  <si>
+    <t>&lt;0.5ppm</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial Unicode MS"/>
+        <family val="2"/>
+        <charset val="136"/>
+      </rPr>
+      <t>≦</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> 10</t>
+    </r>
+  </si>
+  <si>
+    <t>DF310E</t>
+  </si>
+  <si>
+    <t>10ppb</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
-    <numFmt numFmtId="176" formatCode="0.000%"/>
-    <numFmt numFmtId="178" formatCode="yyyy/m/d;@"/>
+    <numFmt numFmtId="164" formatCode="0.000%"/>
+    <numFmt numFmtId="165" formatCode="yyyy/m/d;@"/>
   </numFmts>
-  <fonts count="10">
+  <fonts count="12">
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
@@ -292,6 +327,18 @@
       <family val="2"/>
       <charset val="136"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <name val="PMingLiu"/>
+      <family val="1"/>
+      <charset val="136"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="136"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -301,7 +348,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="11">
+  <borders count="13">
     <border>
       <left/>
       <right/>
@@ -433,11 +480,37 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -453,12 +526,6 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -471,14 +538,17 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="178" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -486,17 +556,14 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="1" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -510,18 +577,30 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="1" fontId="9" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="1" fontId="9" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="11" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="4" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="一般" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -611,9 +690,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 佈景主題">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -651,9 +730,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -686,26 +765,9 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -738,26 +800,9 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -935,29 +980,29 @@
     <outlinePr summaryBelow="0" summaryRight="0"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:Y970"/>
+  <dimension ref="A1:Y971"/>
   <sheetViews>
     <sheetView tabSelected="1" view="pageBreakPreview" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
       <selection activeCell="E15" sqref="E15:F15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.23046875" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="11.25" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="3.4609375" customWidth="1"/>
-    <col min="2" max="2" width="12.61328125" customWidth="1"/>
-    <col min="3" max="3" width="5.61328125" customWidth="1"/>
-    <col min="4" max="4" width="6.4609375" customWidth="1"/>
-    <col min="5" max="5" width="9.765625" customWidth="1"/>
-    <col min="6" max="6" width="6.23046875" customWidth="1"/>
-    <col min="7" max="7" width="5.84375" customWidth="1"/>
-    <col min="8" max="8" width="12.15234375" customWidth="1"/>
-    <col min="9" max="9" width="12.61328125" customWidth="1"/>
-    <col min="10" max="10" width="5.4609375" customWidth="1"/>
-    <col min="11" max="11" width="4.4609375" customWidth="1"/>
-    <col min="12" max="12" width="11.61328125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="3.5" customWidth="1"/>
+    <col min="2" max="2" width="12.625" customWidth="1"/>
+    <col min="3" max="3" width="5.625" customWidth="1"/>
+    <col min="4" max="4" width="6.5" customWidth="1"/>
+    <col min="5" max="5" width="9.75" customWidth="1"/>
+    <col min="6" max="6" width="6.25" customWidth="1"/>
+    <col min="7" max="7" width="5.875" customWidth="1"/>
+    <col min="8" max="8" width="18.375" customWidth="1"/>
+    <col min="9" max="9" width="12.625" customWidth="1"/>
+    <col min="10" max="10" width="5.5" customWidth="1"/>
+    <col min="11" max="11" width="4.5" customWidth="1"/>
+    <col min="12" max="12" width="11.625" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="4" customWidth="1"/>
-    <col min="14" max="14" width="4.4609375" customWidth="1"/>
-    <col min="15" max="15" width="4.61328125" customWidth="1"/>
+    <col min="14" max="14" width="4.5" customWidth="1"/>
+    <col min="15" max="15" width="4.625" customWidth="1"/>
     <col min="16" max="19" width="9" customWidth="1"/>
     <col min="20" max="25" width="8" customWidth="1"/>
   </cols>
@@ -1018,16 +1063,16 @@
     </row>
     <row r="3" spans="1:25" ht="21" customHeight="1">
       <c r="A3" s="1"/>
-      <c r="B3" s="18" t="s">
+      <c r="B3" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="19"/>
-      <c r="D3" s="19"/>
-      <c r="E3" s="19"/>
-      <c r="F3" s="19"/>
-      <c r="G3" s="19"/>
-      <c r="H3" s="19"/>
-      <c r="I3" s="19"/>
+      <c r="C3" s="16"/>
+      <c r="D3" s="16"/>
+      <c r="E3" s="16"/>
+      <c r="F3" s="16"/>
+      <c r="G3" s="16"/>
+      <c r="H3" s="16"/>
+      <c r="I3" s="16"/>
       <c r="J3" s="1"/>
       <c r="K3" s="1"/>
       <c r="L3" s="1"/>
@@ -1047,16 +1092,16 @@
     </row>
     <row r="4" spans="1:25" ht="21" customHeight="1">
       <c r="A4" s="1"/>
-      <c r="B4" s="18" t="s">
+      <c r="B4" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="19"/>
-      <c r="D4" s="19"/>
-      <c r="E4" s="19"/>
-      <c r="F4" s="19"/>
-      <c r="G4" s="19"/>
-      <c r="H4" s="19"/>
-      <c r="I4" s="19"/>
+      <c r="C4" s="16"/>
+      <c r="D4" s="16"/>
+      <c r="E4" s="16"/>
+      <c r="F4" s="16"/>
+      <c r="G4" s="16"/>
+      <c r="H4" s="16"/>
+      <c r="I4" s="16"/>
       <c r="J4" s="1"/>
       <c r="K4" s="1"/>
       <c r="L4" s="1"/>
@@ -1108,7 +1153,7 @@
       </c>
       <c r="C6" s="3"/>
       <c r="D6" s="3"/>
-      <c r="E6" s="7" t="s">
+      <c r="E6" s="5" t="s">
         <v>7</v>
       </c>
       <c r="F6" s="3" t="s">
@@ -1143,16 +1188,16 @@
       </c>
       <c r="C7" s="3"/>
       <c r="D7" s="3"/>
-      <c r="E7" s="11">
+      <c r="E7" s="9">
         <f ca="1">TODAY()</f>
-        <v>44988</v>
+        <v>45665</v>
       </c>
       <c r="F7" s="3" t="s">
         <v>4</v>
       </c>
       <c r="G7" s="3"/>
       <c r="H7" s="3"/>
-      <c r="I7" s="12">
+      <c r="I7" s="10">
         <v>0.99999000000000005</v>
       </c>
       <c r="J7" s="1"/>
@@ -1201,21 +1246,21 @@
     </row>
     <row r="9" spans="1:25" ht="16.5" customHeight="1">
       <c r="A9" s="1"/>
-      <c r="B9" s="13" t="s">
+      <c r="B9" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="C9" s="13" t="s">
+      <c r="C9" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="D9" s="13"/>
-      <c r="E9" s="20" t="s">
+      <c r="D9" s="11"/>
+      <c r="E9" s="18" t="s">
         <v>19</v>
       </c>
-      <c r="F9" s="21"/>
-      <c r="G9" s="20" t="s">
+      <c r="F9" s="19"/>
+      <c r="G9" s="18" t="s">
         <v>5</v>
       </c>
-      <c r="H9" s="21"/>
+      <c r="H9" s="19"/>
       <c r="I9" s="17" t="s">
         <v>6</v>
       </c>
@@ -1238,13 +1283,13 @@
     </row>
     <row r="10" spans="1:25" ht="30" customHeight="1">
       <c r="A10" s="1"/>
-      <c r="B10" s="13"/>
-      <c r="C10" s="13"/>
-      <c r="D10" s="13"/>
-      <c r="E10" s="22"/>
-      <c r="F10" s="23"/>
-      <c r="G10" s="22"/>
-      <c r="H10" s="23"/>
+      <c r="B10" s="11"/>
+      <c r="C10" s="11"/>
+      <c r="D10" s="11"/>
+      <c r="E10" s="20"/>
+      <c r="F10" s="21"/>
+      <c r="G10" s="20"/>
+      <c r="H10" s="21"/>
       <c r="I10" s="17"/>
       <c r="J10" s="4"/>
       <c r="K10" s="4"/>
@@ -1265,22 +1310,22 @@
     </row>
     <row r="11" spans="1:25" ht="28.5" customHeight="1">
       <c r="A11" s="1"/>
-      <c r="B11" s="10" t="s">
+      <c r="B11" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="C11" s="25" t="s">
+      <c r="C11" s="22" t="s">
         <v>18</v>
       </c>
-      <c r="D11" s="26"/>
-      <c r="E11" s="16" t="s">
+      <c r="D11" s="23"/>
+      <c r="E11" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="F11" s="16"/>
-      <c r="G11" s="14" t="s">
+      <c r="F11" s="12"/>
+      <c r="G11" s="13" t="s">
         <v>25</v>
       </c>
-      <c r="H11" s="15"/>
-      <c r="I11" s="9" t="s">
+      <c r="H11" s="14"/>
+      <c r="I11" s="7" t="s">
         <v>16</v>
       </c>
       <c r="J11" s="4"/>
@@ -1302,22 +1347,22 @@
     </row>
     <row r="12" spans="1:25" ht="28.5" customHeight="1">
       <c r="A12" s="1"/>
-      <c r="B12" s="10" t="s">
+      <c r="B12" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="C12" s="13" t="s">
+      <c r="C12" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="D12" s="13"/>
+      <c r="D12" s="11"/>
       <c r="E12" s="24" t="s">
         <v>26</v>
       </c>
-      <c r="F12" s="16"/>
-      <c r="G12" s="14" t="s">
+      <c r="F12" s="12"/>
+      <c r="G12" s="13" t="s">
         <v>25</v>
       </c>
-      <c r="H12" s="15"/>
-      <c r="I12" s="9" t="s">
+      <c r="H12" s="14"/>
+      <c r="I12" s="7" t="s">
         <v>16</v>
       </c>
       <c r="J12" s="4"/>
@@ -1339,22 +1384,22 @@
     </row>
     <row r="13" spans="1:25" ht="28.5" customHeight="1">
       <c r="A13" s="1"/>
-      <c r="B13" s="10" t="s">
+      <c r="B13" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="C13" s="13" t="s">
+      <c r="C13" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="D13" s="13"/>
-      <c r="E13" s="16" t="s">
+      <c r="D13" s="11"/>
+      <c r="E13" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="F13" s="16"/>
-      <c r="G13" s="14" t="s">
+      <c r="F13" s="12"/>
+      <c r="G13" s="13" t="s">
         <v>25</v>
       </c>
-      <c r="H13" s="15"/>
-      <c r="I13" s="9" t="s">
+      <c r="H13" s="14"/>
+      <c r="I13" s="7" t="s">
         <v>16</v>
       </c>
       <c r="J13" s="4"/>
@@ -1376,22 +1421,22 @@
     </row>
     <row r="14" spans="1:25" ht="28.5" customHeight="1">
       <c r="A14" s="1"/>
-      <c r="B14" s="10" t="s">
+      <c r="B14" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="C14" s="13" t="s">
+      <c r="C14" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="D14" s="13"/>
-      <c r="E14" s="16" t="s">
+      <c r="D14" s="11"/>
+      <c r="E14" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="F14" s="16"/>
-      <c r="G14" s="14" t="s">
+      <c r="F14" s="12"/>
+      <c r="G14" s="13" t="s">
         <v>25</v>
       </c>
-      <c r="H14" s="15"/>
-      <c r="I14" s="9" t="s">
+      <c r="H14" s="14"/>
+      <c r="I14" s="7" t="s">
         <v>16</v>
       </c>
       <c r="J14" s="4"/>
@@ -1413,22 +1458,22 @@
     </row>
     <row r="15" spans="1:25" ht="28.5" customHeight="1">
       <c r="A15" s="1"/>
-      <c r="B15" s="10" t="s">
+      <c r="B15" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="C15" s="13" t="s">
+      <c r="C15" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="D15" s="13"/>
-      <c r="E15" s="16" t="s">
+      <c r="D15" s="11"/>
+      <c r="E15" s="12" t="s">
         <v>24</v>
       </c>
-      <c r="F15" s="16"/>
-      <c r="G15" s="14" t="s">
+      <c r="F15" s="12"/>
+      <c r="G15" s="13" t="s">
         <v>25</v>
       </c>
-      <c r="H15" s="15"/>
-      <c r="I15" s="9" t="s">
+      <c r="H15" s="14"/>
+      <c r="I15" s="7" t="s">
         <v>27</v>
       </c>
       <c r="J15" s="4"/>
@@ -1450,22 +1495,22 @@
     </row>
     <row r="16" spans="1:25" ht="28.5" customHeight="1">
       <c r="A16" s="1"/>
-      <c r="B16" s="8" t="s">
+      <c r="B16" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="C16" s="13" t="s">
+      <c r="C16" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="D16" s="13"/>
-      <c r="E16" s="16" t="s">
+      <c r="D16" s="11"/>
+      <c r="E16" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="F16" s="16"/>
-      <c r="G16" s="14" t="s">
+      <c r="F16" s="12"/>
+      <c r="G16" s="13" t="s">
         <v>25</v>
       </c>
-      <c r="H16" s="15"/>
-      <c r="I16" s="9" t="s">
+      <c r="H16" s="14"/>
+      <c r="I16" s="7" t="s">
         <v>16</v>
       </c>
       <c r="J16" s="1"/>
@@ -1485,16 +1530,26 @@
       <c r="X16" s="1"/>
       <c r="Y16" s="1"/>
     </row>
-    <row r="17" spans="1:25" ht="16.5" customHeight="1">
+    <row r="17" spans="1:25" ht="28.5" customHeight="1">
       <c r="A17" s="1"/>
-      <c r="B17" s="1"/>
-      <c r="C17" s="1"/>
-      <c r="D17" s="5"/>
-      <c r="E17" s="5"/>
-      <c r="F17" s="5"/>
-      <c r="G17" s="5"/>
-      <c r="H17" s="5"/>
-      <c r="I17" s="6"/>
+      <c r="B17" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="C17" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="D17" s="11"/>
+      <c r="E17" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="F17" s="12"/>
+      <c r="G17" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="H17" s="14"/>
+      <c r="I17" s="7" t="s">
+        <v>16</v>
+      </c>
       <c r="J17" s="1"/>
       <c r="K17" s="1"/>
       <c r="L17" s="1"/>
@@ -1512,59 +1567,71 @@
       <c r="X17" s="1"/>
       <c r="Y17" s="1"/>
     </row>
-    <row r="18" spans="1:25" ht="16.5" customHeight="1">
-      <c r="A18" s="4"/>
-      <c r="B18" s="4"/>
-      <c r="C18" s="4"/>
-      <c r="D18" s="4"/>
-      <c r="E18" s="4"/>
-      <c r="F18" s="4"/>
-      <c r="G18" s="4"/>
-      <c r="H18" s="4"/>
-      <c r="I18" s="4"/>
-      <c r="J18" s="4"/>
-      <c r="K18" s="4"/>
-      <c r="L18" s="4"/>
-      <c r="M18" s="4"/>
-      <c r="N18" s="4"/>
-      <c r="O18" s="4"/>
-      <c r="P18" s="4"/>
-      <c r="Q18" s="4"/>
-      <c r="R18" s="4"/>
-      <c r="S18" s="4"/>
-      <c r="T18" s="4"/>
-      <c r="U18" s="4"/>
-      <c r="V18" s="4"/>
-      <c r="W18" s="4"/>
-      <c r="X18" s="4"/>
-      <c r="Y18" s="4"/>
+    <row r="18" spans="1:25" ht="28.5" customHeight="1">
+      <c r="A18" s="1"/>
+      <c r="B18" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="C18" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="D18" s="25" t="s">
+        <v>33</v>
+      </c>
+      <c r="E18" s="26" t="s">
+        <v>34</v>
+      </c>
+      <c r="F18" s="27"/>
+      <c r="G18" s="13" t="s">
+        <v>35</v>
+      </c>
+      <c r="H18" s="14"/>
+      <c r="I18" s="28" t="s">
+        <v>36</v>
+      </c>
+      <c r="J18" s="1"/>
+      <c r="K18" s="1"/>
+      <c r="L18" s="1"/>
+      <c r="M18" s="1"/>
+      <c r="N18" s="1"/>
+      <c r="O18" s="1"/>
+      <c r="P18" s="1"/>
+      <c r="Q18" s="1"/>
+      <c r="R18" s="1"/>
+      <c r="S18" s="1"/>
+      <c r="T18" s="1"/>
+      <c r="U18" s="1"/>
+      <c r="V18" s="1"/>
+      <c r="W18" s="1"/>
+      <c r="X18" s="1"/>
+      <c r="Y18" s="1"/>
     </row>
     <row r="19" spans="1:25" ht="16.5" customHeight="1">
-      <c r="A19" s="1"/>
-      <c r="B19" s="1"/>
-      <c r="C19" s="1"/>
-      <c r="D19" s="1"/>
-      <c r="E19" s="1"/>
-      <c r="F19" s="1"/>
-      <c r="G19" s="1"/>
-      <c r="H19" s="1"/>
-      <c r="I19" s="1"/>
-      <c r="J19" s="1"/>
-      <c r="K19" s="1"/>
-      <c r="L19" s="1"/>
-      <c r="M19" s="1"/>
-      <c r="N19" s="1"/>
-      <c r="O19" s="1"/>
-      <c r="P19" s="1"/>
-      <c r="Q19" s="1"/>
-      <c r="R19" s="1"/>
-      <c r="S19" s="1"/>
-      <c r="T19" s="1"/>
-      <c r="U19" s="1"/>
-      <c r="V19" s="1"/>
-      <c r="W19" s="1"/>
-      <c r="X19" s="1"/>
-      <c r="Y19" s="1"/>
+      <c r="A19" s="4"/>
+      <c r="B19" s="4"/>
+      <c r="C19" s="4"/>
+      <c r="D19" s="4"/>
+      <c r="E19" s="4"/>
+      <c r="F19" s="4"/>
+      <c r="G19" s="4"/>
+      <c r="H19" s="4"/>
+      <c r="I19" s="4"/>
+      <c r="J19" s="4"/>
+      <c r="K19" s="4"/>
+      <c r="L19" s="4"/>
+      <c r="M19" s="4"/>
+      <c r="N19" s="4"/>
+      <c r="O19" s="4"/>
+      <c r="P19" s="4"/>
+      <c r="Q19" s="4"/>
+      <c r="R19" s="4"/>
+      <c r="S19" s="4"/>
+      <c r="T19" s="4"/>
+      <c r="U19" s="4"/>
+      <c r="V19" s="4"/>
+      <c r="W19" s="4"/>
+      <c r="X19" s="4"/>
+      <c r="Y19" s="4"/>
     </row>
     <row r="20" spans="1:25" ht="16.5" customHeight="1">
       <c r="A20" s="1"/>
@@ -27243,19 +27310,38 @@
       <c r="X970" s="1"/>
       <c r="Y970" s="1"/>
     </row>
+    <row r="971" spans="1:25" ht="16.5" customHeight="1">
+      <c r="A971" s="1"/>
+      <c r="B971" s="1"/>
+      <c r="C971" s="1"/>
+      <c r="D971" s="1"/>
+      <c r="E971" s="1"/>
+      <c r="F971" s="1"/>
+      <c r="G971" s="1"/>
+      <c r="H971" s="1"/>
+      <c r="I971" s="1"/>
+      <c r="J971" s="1"/>
+      <c r="K971" s="1"/>
+      <c r="L971" s="1"/>
+      <c r="M971" s="1"/>
+      <c r="N971" s="1"/>
+      <c r="O971" s="1"/>
+      <c r="P971" s="1"/>
+      <c r="Q971" s="1"/>
+      <c r="R971" s="1"/>
+      <c r="S971" s="1"/>
+      <c r="T971" s="1"/>
+      <c r="U971" s="1"/>
+      <c r="V971" s="1"/>
+      <c r="W971" s="1"/>
+      <c r="X971" s="1"/>
+      <c r="Y971" s="1"/>
+    </row>
   </sheetData>
-  <mergeCells count="25">
-    <mergeCell ref="C15:D15"/>
-    <mergeCell ref="E15:F15"/>
-    <mergeCell ref="G15:H15"/>
-    <mergeCell ref="E16:F16"/>
-    <mergeCell ref="B3:I3"/>
-    <mergeCell ref="B4:I4"/>
-    <mergeCell ref="I9:I10"/>
-    <mergeCell ref="C9:D10"/>
-    <mergeCell ref="B9:B10"/>
-    <mergeCell ref="G9:H10"/>
-    <mergeCell ref="C16:D16"/>
+  <mergeCells count="31">
+    <mergeCell ref="C18:D18"/>
+    <mergeCell ref="E18:F18"/>
+    <mergeCell ref="G18:H18"/>
     <mergeCell ref="C12:D12"/>
     <mergeCell ref="C13:D13"/>
     <mergeCell ref="C14:D14"/>
@@ -27263,13 +27349,27 @@
     <mergeCell ref="G16:H16"/>
     <mergeCell ref="G13:H13"/>
     <mergeCell ref="G14:H14"/>
-    <mergeCell ref="E9:F10"/>
     <mergeCell ref="G11:H11"/>
     <mergeCell ref="G12:H12"/>
     <mergeCell ref="E12:F12"/>
     <mergeCell ref="E11:F11"/>
     <mergeCell ref="E13:F13"/>
     <mergeCell ref="E14:F14"/>
+    <mergeCell ref="B3:I3"/>
+    <mergeCell ref="B4:I4"/>
+    <mergeCell ref="I9:I10"/>
+    <mergeCell ref="C9:D10"/>
+    <mergeCell ref="B9:B10"/>
+    <mergeCell ref="G9:H10"/>
+    <mergeCell ref="E9:F10"/>
+    <mergeCell ref="C17:D17"/>
+    <mergeCell ref="E17:F17"/>
+    <mergeCell ref="G17:H17"/>
+    <mergeCell ref="C15:D15"/>
+    <mergeCell ref="E15:F15"/>
+    <mergeCell ref="G15:H15"/>
+    <mergeCell ref="E16:F16"/>
+    <mergeCell ref="C16:D16"/>
   </mergeCells>
   <phoneticPr fontId="8" type="noConversion"/>
   <printOptions horizontalCentered="1"/>

</xml_diff>